<commit_message>
Updates on Portfolio Simulation
</commit_message>
<xml_diff>
--- a/Entertainment.xlsx
+++ b/Entertainment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1.Finance\Anaylsen\Sectors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52559300-763D-4268-BA9A-269B25CECC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D663EAF1-64A1-472A-BDB0-F20EFA9FC721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="225" yWindow="1950" windowWidth="38175" windowHeight="15240" xr2:uid="{E414CA5C-78F9-4930-AC5C-325CFFA496F2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21060" xr2:uid="{E414CA5C-78F9-4930-AC5C-325CFFA496F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -1917,7 +1917,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2282,7 +2282,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3502,10 +3502,10 @@
   <dimension ref="A1:W224"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="196" zoomScaleNormal="196" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>